<commit_message>
My test successfully enters attendance records into the database.
</commit_message>
<xml_diff>
--- a/src/test/resources/database_input.xlsx
+++ b/src/test/resources/database_input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>username</t>
   </si>
@@ -108,12 +108,6 @@
     <t>userToken</t>
   </si>
   <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>goodbye</t>
-  </si>
-  <si>
     <t>KeyColumn</t>
   </si>
   <si>
@@ -145,6 +139,18 @@
   </si>
   <si>
     <t>superAdmin</t>
+  </si>
+  <si>
+    <t>My name is Jonas</t>
+  </si>
+  <si>
+    <t>I'm carrying the will</t>
+  </si>
+  <si>
+    <t>02/03/2017</t>
+  </si>
+  <si>
+    <t>01/22/2017</t>
   </si>
 </sst>
 </file>
@@ -188,9 +194,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,20 +495,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -542,27 +550,45 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>11</v>
       </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>16</v>
       </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
@@ -654,10 +680,10 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -665,10 +691,10 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -676,10 +702,10 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -687,10 +713,10 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -698,10 +724,10 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -719,7 +745,7 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
making changes related to new graduation date field.
</commit_message>
<xml_diff>
--- a/src/test/resources/database_input.xlsx
+++ b/src/test/resources/database_input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>username</t>
   </si>
@@ -33,12 +33,6 @@
     <t>batchType</t>
   </si>
   <si>
-    <t>attendance</t>
-  </si>
-  <si>
-    <t>tasks</t>
-  </si>
-  <si>
     <t>userRole</t>
   </si>
   <si>
@@ -151,6 +145,15 @@
   </si>
   <si>
     <t>01/22/2017</t>
+  </si>
+  <si>
+    <t>graduationDate</t>
+  </si>
+  <si>
+    <t>01/02/2017</t>
+  </si>
+  <si>
+    <t>01/06/2017</t>
   </si>
 </sst>
 </file>
@@ -194,11 +197,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -508,7 +512,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -543,23 +547,23 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -570,7 +574,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -581,98 +585,98 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -680,10 +684,10 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -691,10 +695,10 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -702,10 +706,10 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -713,10 +717,10 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -724,31 +728,32 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>5</v>
       </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" t="s">
-        <v>23</v>
+        <v>43</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>